<commit_message>
working version for me
</commit_message>
<xml_diff>
--- a/src/main/resources/excelimport/WM2018.xlsx
+++ b/src/main/resources/excelimport/WM2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbelmokhtar\Desktop\Nouveau dossier\GIthub\fredbet\src\main\resources\excelimport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA1ACC81-D06C-4D3A-9384-855E8603DCF2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC00A3FF-A594-4E13-A573-40E373B9E187}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,22 @@
     <sheet name="Countries" sheetId="2" r:id="rId2"/>
     <sheet name="Groups" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="244">
   <si>
     <t>Country 1</t>
   </si>
@@ -50,9 +55,6 @@
     <t>GERMANY</t>
   </si>
   <si>
-    <t>GROUP_A</t>
-  </si>
-  <si>
     <t>ALBANIA</t>
   </si>
   <si>
@@ -677,27 +679,6 @@
     <t>VENEZUELA</t>
   </si>
   <si>
-    <t>GROUP_B</t>
-  </si>
-  <si>
-    <t>GROUP_C</t>
-  </si>
-  <si>
-    <t>GROUP_D</t>
-  </si>
-  <si>
-    <t>GROUP_E</t>
-  </si>
-  <si>
-    <t>GROUP_F</t>
-  </si>
-  <si>
-    <t>GROUP_G</t>
-  </si>
-  <si>
-    <t>GROUP_H</t>
-  </si>
-  <si>
     <t>ROUND_OF_SIXTEEN</t>
   </si>
   <si>
@@ -713,117 +694,6 @@
     <t>GAME_FOR_THIRD</t>
   </si>
   <si>
-    <t>Luschniki</t>
-  </si>
-  <si>
-    <t>Jekaterinburg</t>
-  </si>
-  <si>
-    <t>Sankt Petersburg</t>
-  </si>
-  <si>
-    <t>Rostow am Don</t>
-  </si>
-  <si>
-    <t>Samara</t>
-  </si>
-  <si>
-    <t>Wolgograd</t>
-  </si>
-  <si>
-    <t>Sotschi</t>
-  </si>
-  <si>
-    <t>Kasan</t>
-  </si>
-  <si>
-    <t>Saransk</t>
-  </si>
-  <si>
-    <t>Kaliningrad</t>
-  </si>
-  <si>
-    <t>Spartak</t>
-  </si>
-  <si>
-    <t>Nischni Nowgorod</t>
-  </si>
-  <si>
-    <t>Moskau</t>
-  </si>
-  <si>
-    <t>Sieger C</t>
-  </si>
-  <si>
-    <t>Zweiter D</t>
-  </si>
-  <si>
-    <t>Sieger A</t>
-  </si>
-  <si>
-    <t>Zweiter B</t>
-  </si>
-  <si>
-    <t>Sieger B</t>
-  </si>
-  <si>
-    <t>Zweiter A</t>
-  </si>
-  <si>
-    <t>Sieger D</t>
-  </si>
-  <si>
-    <t>Zweiter C</t>
-  </si>
-  <si>
-    <t>Sieger E</t>
-  </si>
-  <si>
-    <t>Zweiter F</t>
-  </si>
-  <si>
-    <t>Sieger G</t>
-  </si>
-  <si>
-    <t>Zweiter H</t>
-  </si>
-  <si>
-    <t>Sieger F</t>
-  </si>
-  <si>
-    <t>Sieger H</t>
-  </si>
-  <si>
-    <t>Zweiter E</t>
-  </si>
-  <si>
-    <t>Zweiter G</t>
-  </si>
-  <si>
-    <t>Sieger A1</t>
-  </si>
-  <si>
-    <t>Zweiter A2</t>
-  </si>
-  <si>
-    <t>Sieger A3</t>
-  </si>
-  <si>
-    <t>Zweiter A4</t>
-  </si>
-  <si>
-    <t>Sieger A5</t>
-  </si>
-  <si>
-    <t>Zweiter A6</t>
-  </si>
-  <si>
-    <t>Sieger A7</t>
-  </si>
-  <si>
-    <t>Zweiter A8</t>
-  </si>
-  <si>
     <t>Sieger HF1</t>
   </si>
   <si>
@@ -846,6 +716,54 @@
   </si>
   <si>
     <t>Sieger VF3</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Bayern Munich</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Atl. Madrid</t>
+  </si>
+  <si>
+    <t>Juventus</t>
+  </si>
+  <si>
+    <t>Schalke</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>Dortmund</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Real Madrid</t>
+  </si>
+  <si>
+    <t>Ajax</t>
+  </si>
+  <si>
+    <t>FC Porto</t>
+  </si>
+  <si>
+    <t>AS Roma</t>
+  </si>
+  <si>
+    <t>Paris SG</t>
+  </si>
+  <si>
+    <t>Manchester Utd</t>
   </si>
 </sst>
 </file>
@@ -901,7 +819,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -917,7 +835,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1213,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E440"/>
+  <dimension ref="A1:E392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,6 +1144,8 @@
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,1135 +1167,479 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D2" s="2">
-        <v>43265.708333333336</v>
-      </c>
-      <c r="E2" t="s">
-        <v>228</v>
+        <v>43515.875</v>
+      </c>
+      <c r="E2" t="str">
+        <f>A2</f>
+        <v>Liverpool</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D3" s="2">
-        <v>43266.583333333336</v>
-      </c>
-      <c r="E3" t="s">
-        <v>229</v>
+        <v>43515.875</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E17" si="0">A3</f>
+        <v>Lyon</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D4" s="2">
-        <v>43270.833333333336</v>
-      </c>
-      <c r="E4" t="s">
-        <v>230</v>
+        <v>43516.875</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Atl. Madrid</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D5" s="2">
-        <v>43271.708333333336</v>
-      </c>
-      <c r="E5" t="s">
-        <v>231</v>
+        <v>43516.875</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Schalke</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D6" s="2">
-        <v>43276.666666666664</v>
-      </c>
-      <c r="E6" t="s">
-        <v>232</v>
+        <v>43529.875</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Dortmund</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
       <c r="D7" s="2">
-        <v>43276.666666666664</v>
-      </c>
-      <c r="E7" t="s">
-        <v>233</v>
+        <v>43529.875</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Real Madrid</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="2">
-        <v>43266.708333333336</v>
-      </c>
-      <c r="E8" t="s">
-        <v>230</v>
+        <v>43530.875</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>FC Porto</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" s="2">
-        <v>43266.833333333336</v>
-      </c>
-      <c r="E9" t="s">
-        <v>234</v>
+        <v>43530.875</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Paris SG</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D10" s="2">
-        <v>43271.583333333336</v>
-      </c>
-      <c r="E10" t="s">
-        <v>228</v>
+        <v>43536.875</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Juventus</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="2">
-        <v>43271.833333333336</v>
-      </c>
-      <c r="E11" t="s">
-        <v>235</v>
+        <v>43536.875</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Manchester City</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="2">
-        <v>43276.833333333336</v>
-      </c>
-      <c r="E12" t="s">
-        <v>236</v>
+        <v>43537.875</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Barcelona</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>228</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="2">
-        <v>43276.833333333336</v>
-      </c>
-      <c r="E13" t="s">
-        <v>237</v>
+        <v>43537.875</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Bayern Munich</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>224</v>
       </c>
       <c r="C14" t="s">
         <v>217</v>
       </c>
       <c r="D14" s="2">
-        <v>43267.5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>235</v>
+        <v>43291.833333333336</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Sieger VF2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
         <v>217</v>
       </c>
       <c r="D15" s="2">
-        <v>43267.75</v>
-      </c>
-      <c r="E15" t="s">
-        <v>236</v>
+        <v>43292.833333333336</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Sieger VF4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D16" s="2">
-        <v>43272.708333333336</v>
-      </c>
-      <c r="E16" t="s">
-        <v>229</v>
+        <v>43296.708333333336</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Sieger HF1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>223</v>
       </c>
       <c r="C17" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D17" s="2">
-        <v>43272.583333333336</v>
-      </c>
-      <c r="E17" t="s">
-        <v>232</v>
+        <v>43295.666666666664</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Verlierer HF1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D18" s="2">
-        <v>43277.666666666664</v>
-      </c>
-      <c r="E18" t="s">
-        <v>228</v>
-      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D19" s="2">
-        <v>43277.666666666664</v>
-      </c>
-      <c r="E19" t="s">
-        <v>234</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>206</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>218</v>
-      </c>
-      <c r="D20" s="2">
-        <v>43267.625</v>
-      </c>
-      <c r="E20" t="s">
-        <v>238</v>
-      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D21" s="2">
-        <v>43267.875</v>
-      </c>
-      <c r="E21" t="s">
-        <v>237</v>
-      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D22" s="2">
-        <v>43272.833333333336</v>
-      </c>
-      <c r="E22" t="s">
-        <v>239</v>
-      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="2">
-        <v>43273.708333333336</v>
-      </c>
-      <c r="E23" t="s">
-        <v>233</v>
-      </c>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>218</v>
-      </c>
-      <c r="D24" s="2">
-        <v>43277.833333333336</v>
-      </c>
-      <c r="E24" t="s">
-        <v>230</v>
-      </c>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" s="2">
-        <v>43277.833333333336</v>
-      </c>
-      <c r="E25" t="s">
-        <v>231</v>
-      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" s="2">
-        <v>43268.583333333336</v>
-      </c>
-      <c r="E26" t="s">
-        <v>231</v>
-      </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>208</v>
-      </c>
-      <c r="B27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>219</v>
-      </c>
-      <c r="D27" s="2">
-        <v>43268.833333333336</v>
-      </c>
-      <c r="E27" t="s">
-        <v>232</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>208</v>
-      </c>
-      <c r="B28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D28" s="2">
-        <v>43273.583333333336</v>
-      </c>
-      <c r="E28" t="s">
-        <v>230</v>
-      </c>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" t="s">
-        <v>219</v>
-      </c>
-      <c r="D29" s="2">
-        <v>43273.833333333336</v>
-      </c>
-      <c r="E29" t="s">
-        <v>237</v>
-      </c>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" t="s">
-        <v>208</v>
-      </c>
-      <c r="C30" t="s">
-        <v>219</v>
-      </c>
-      <c r="D30" s="2">
-        <v>43278.833333333336</v>
-      </c>
-      <c r="E30" t="s">
-        <v>238</v>
-      </c>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" t="s">
-        <v>219</v>
-      </c>
-      <c r="D31" s="2">
-        <v>43278.833333333336</v>
-      </c>
-      <c r="E31" t="s">
-        <v>239</v>
-      </c>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" t="s">
-        <v>220</v>
-      </c>
-      <c r="D32" s="2">
-        <v>43268.708333333336</v>
-      </c>
-      <c r="E32" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" t="s">
-        <v>220</v>
-      </c>
-      <c r="D33" s="2">
-        <v>43269.583333333336</v>
-      </c>
-      <c r="E33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" t="s">
-        <v>220</v>
-      </c>
-      <c r="D34" s="2">
-        <v>43274.833333333336</v>
-      </c>
-      <c r="E34" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" t="s">
-        <v>182</v>
-      </c>
-      <c r="C35" t="s">
-        <v>220</v>
-      </c>
-      <c r="D35" s="2">
-        <v>43274.708333333336</v>
-      </c>
-      <c r="E35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>182</v>
-      </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" t="s">
-        <v>220</v>
-      </c>
-      <c r="D36" s="2">
-        <v>43278.666666666664</v>
-      </c>
-      <c r="E36" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="2">
-        <v>43278.666666666664</v>
-      </c>
-      <c r="E37" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" t="s">
-        <v>221</v>
-      </c>
-      <c r="D38" s="2">
-        <v>43269.708333333336</v>
-      </c>
-      <c r="E38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" t="s">
-        <v>221</v>
-      </c>
-      <c r="D39" s="2">
-        <v>43269.833333333336</v>
-      </c>
-      <c r="E39" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>221</v>
-      </c>
-      <c r="D40" s="2">
-        <v>43274.583333333336</v>
-      </c>
-      <c r="E40" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" t="s">
-        <v>221</v>
-      </c>
-      <c r="D41" s="2">
-        <v>43275.583333333336</v>
-      </c>
-      <c r="E41" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>221</v>
-      </c>
-      <c r="D42" s="2">
-        <v>43279.833333333336</v>
-      </c>
-      <c r="E42" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D43" s="2">
-        <v>43279.833333333336</v>
-      </c>
-      <c r="E43" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" t="s">
-        <v>222</v>
-      </c>
-      <c r="D44" s="2">
-        <v>43270.708333333336</v>
-      </c>
-      <c r="E44" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>210</v>
-      </c>
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" t="s">
-        <v>222</v>
-      </c>
-      <c r="D45" s="2">
-        <v>43270.583333333336</v>
-      </c>
-      <c r="E45" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" t="s">
-        <v>222</v>
-      </c>
-      <c r="D46" s="2">
-        <v>43275.708333333336</v>
-      </c>
-      <c r="E46" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" t="s">
-        <v>210</v>
-      </c>
-      <c r="C47" t="s">
-        <v>222</v>
-      </c>
-      <c r="D47" s="2">
-        <v>43275.833333333336</v>
-      </c>
-      <c r="E47" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" t="s">
-        <v>210</v>
-      </c>
-      <c r="C48" t="s">
-        <v>222</v>
-      </c>
-      <c r="D48" s="2">
-        <v>43279.666666666664</v>
-      </c>
-      <c r="E48" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" t="s">
-        <v>222</v>
-      </c>
-      <c r="D49" s="2">
-        <v>43279.666666666664</v>
-      </c>
-      <c r="E49" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>241</v>
-      </c>
-      <c r="B50" t="s">
-        <v>242</v>
-      </c>
-      <c r="C50" t="s">
-        <v>223</v>
-      </c>
-      <c r="D50" s="2">
-        <v>43281.666666666664</v>
-      </c>
-      <c r="E50" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>243</v>
-      </c>
-      <c r="B51" t="s">
-        <v>244</v>
-      </c>
-      <c r="C51" t="s">
-        <v>223</v>
-      </c>
-      <c r="D51" s="2">
-        <v>43281.833333333336</v>
-      </c>
-      <c r="E51" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>245</v>
-      </c>
-      <c r="B52" t="s">
-        <v>246</v>
-      </c>
-      <c r="C52" t="s">
-        <v>223</v>
-      </c>
-      <c r="D52" s="2">
-        <v>43282.666666666664</v>
-      </c>
-      <c r="E52" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>247</v>
-      </c>
-      <c r="B53" t="s">
-        <v>248</v>
-      </c>
-      <c r="C53" t="s">
-        <v>223</v>
-      </c>
-      <c r="D53" s="2">
-        <v>43282.833333333336</v>
-      </c>
-      <c r="E53" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>249</v>
-      </c>
-      <c r="B54" t="s">
-        <v>250</v>
-      </c>
-      <c r="C54" t="s">
-        <v>223</v>
-      </c>
-      <c r="D54" s="2">
-        <v>43283.666666666664</v>
-      </c>
-      <c r="E54" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>251</v>
-      </c>
-      <c r="B55" t="s">
-        <v>252</v>
-      </c>
-      <c r="C55" t="s">
-        <v>223</v>
-      </c>
-      <c r="D55" s="2">
-        <v>43283.833333333336</v>
-      </c>
-      <c r="E55" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>253</v>
-      </c>
-      <c r="B56" t="s">
-        <v>255</v>
-      </c>
-      <c r="C56" t="s">
-        <v>223</v>
-      </c>
-      <c r="D56" s="2">
-        <v>43284.666666666664</v>
-      </c>
-      <c r="E56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>254</v>
-      </c>
-      <c r="B57" t="s">
-        <v>256</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
-      </c>
-      <c r="D57" s="2">
-        <v>43284.833333333336</v>
-      </c>
-      <c r="E57" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>257</v>
-      </c>
-      <c r="B58" t="s">
-        <v>258</v>
-      </c>
-      <c r="C58" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" s="2">
-        <v>43287.666666666664</v>
-      </c>
-      <c r="E58" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>259</v>
-      </c>
-      <c r="B59" t="s">
-        <v>260</v>
-      </c>
-      <c r="C59" t="s">
-        <v>224</v>
-      </c>
-      <c r="D59" s="2">
-        <v>43288.833333333336</v>
-      </c>
-      <c r="E59" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>261</v>
-      </c>
-      <c r="B60" t="s">
-        <v>262</v>
-      </c>
-      <c r="C60" t="s">
-        <v>224</v>
-      </c>
-      <c r="D60" s="2">
-        <v>43287.833333333336</v>
-      </c>
-      <c r="E60" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>263</v>
-      </c>
-      <c r="B61" t="s">
-        <v>264</v>
-      </c>
-      <c r="C61" t="s">
-        <v>224</v>
-      </c>
-      <c r="D61" s="2">
-        <v>43288.666666666664</v>
-      </c>
-      <c r="E61" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>270</v>
-      </c>
-      <c r="B62" t="s">
-        <v>269</v>
-      </c>
-      <c r="C62" t="s">
-        <v>225</v>
-      </c>
-      <c r="D62" s="2">
-        <v>43291.833333333336</v>
-      </c>
-      <c r="E62" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>271</v>
-      </c>
-      <c r="B63" t="s">
-        <v>272</v>
-      </c>
-      <c r="C63" t="s">
-        <v>225</v>
-      </c>
-      <c r="D63" s="2">
-        <v>43292.833333333336</v>
-      </c>
-      <c r="E63" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>265</v>
-      </c>
-      <c r="B64" t="s">
-        <v>266</v>
-      </c>
-      <c r="C64" t="s">
-        <v>226</v>
-      </c>
-      <c r="D64" s="2">
-        <v>43296.708333333336</v>
-      </c>
-      <c r="E64" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>267</v>
-      </c>
-      <c r="B65" t="s">
-        <v>268</v>
-      </c>
-      <c r="C65" t="s">
-        <v>227</v>
-      </c>
-      <c r="D65" s="2">
-        <v>43295.666666666664</v>
-      </c>
-      <c r="E65" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
@@ -3313,150 +2577,6 @@
     </row>
     <row r="392" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D392" s="2"/>
-    </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D393" s="2"/>
-    </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D394" s="2"/>
-    </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D395" s="2"/>
-    </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D396" s="2"/>
-    </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D397" s="2"/>
-    </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D398" s="2"/>
-    </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D399" s="2"/>
-    </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D400" s="2"/>
-    </row>
-    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D401" s="2"/>
-    </row>
-    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D402" s="2"/>
-    </row>
-    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D403" s="2"/>
-    </row>
-    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D404" s="2"/>
-    </row>
-    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D405" s="2"/>
-    </row>
-    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D406" s="2"/>
-    </row>
-    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D407" s="2"/>
-    </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D408" s="2"/>
-    </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D409" s="2"/>
-    </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D410" s="2"/>
-    </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D411" s="2"/>
-    </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D412" s="2"/>
-    </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D413" s="2"/>
-    </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D414" s="2"/>
-    </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D415" s="2"/>
-    </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D416" s="2"/>
-    </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D417" s="2"/>
-    </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D418" s="2"/>
-    </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D419" s="2"/>
-    </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D420" s="2"/>
-    </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D421" s="2"/>
-    </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D422" s="2"/>
-    </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D423" s="2"/>
-    </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D424" s="2"/>
-    </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D425" s="2"/>
-    </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D426" s="2"/>
-    </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D427" s="2"/>
-    </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D428" s="2"/>
-    </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D429" s="2"/>
-    </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D430" s="2"/>
-    </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D431" s="2"/>
-    </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D432" s="2"/>
-    </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D433" s="2"/>
-    </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D434" s="2"/>
-    </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D435" s="2"/>
-    </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D436" s="2"/>
-    </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D437" s="2"/>
-    </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D438" s="2"/>
-    </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D439" s="2"/>
-    </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D440" s="2"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
@@ -3469,13 +2589,13 @@
           <x14:formula1>
             <xm:f>Countries!$A$1:$A$210</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:B440</xm:sqref>
+          <xm:sqref>A2:B392</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>Groups!$A$1:$A$13</xm:f>
+            <xm:f>Groups!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C440</xm:sqref>
+          <xm:sqref>C2:C392</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3487,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A210"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,97 +2618,97 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -3598,272 +2718,272 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
@@ -3873,677 +2993,677 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4556,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4569,7 +3689,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -4590,46 +3710,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>